<commit_message>
Criacao de arquivo e escolha de colunas para o arquivo funcionando
(falta concatenar o endereco)
</commit_message>
<xml_diff>
--- a/Rotas.xlsx
+++ b/Rotas.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="96">
   <si>
     <t>DATA</t>
   </si>
@@ -133,7 +133,7 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>Campinas</t>
+    <t>Araraquara</t>
   </si>
   <si>
     <t>AFNM</t>
@@ -173,9 +173,6 @@
   </si>
   <si>
     <t>Vila Santa Catarina</t>
-  </si>
-  <si>
-    <t>Bauru</t>
   </si>
   <si>
     <t>ABERB</t>
@@ -308,7 +305,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <fonts count="5">
+  <fonts count="4">
     <font>
       <sz val="11.0"/>
       <color theme="1"/>
@@ -328,11 +325,6 @@
       <sz val="11.0"/>
       <color theme="1"/>
       <name val="Calibri"/>
-    </font>
-    <font>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -360,11 +352,11 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf quotePrefix="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
@@ -753,7 +745,7 @@
       </c>
       <c r="J2" s="3">
         <f t="shared" ref="J2:J11" si="1">RANDBETWEEN(11111,55555)</f>
-        <v>49375</v>
+        <v>12910</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>39</v>
@@ -767,9 +759,7 @@
       <c r="N2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="O2" s="2" t="s">
-        <v>39</v>
-      </c>
+      <c r="O2" s="2"/>
       <c r="P2" s="2" t="s">
         <v>39</v>
       </c>
@@ -779,10 +769,10 @@
       <c r="R2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="S2" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="T2" s="4" t="s">
+      <c r="T2" s="5" t="s">
         <v>41</v>
       </c>
       <c r="U2" s="2" t="s">
@@ -800,7 +790,7 @@
       <c r="Y2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="Z2" s="5" t="s">
+      <c r="Z2" s="2" t="s">
         <v>39</v>
       </c>
       <c r="AA2" s="2" t="s">
@@ -808,7 +798,7 @@
       </c>
       <c r="AB2" s="6">
         <f t="shared" ref="AB2:AB11" si="2">RANDBETWEEN(111,200)</f>
-        <v>184</v>
+        <v>148</v>
       </c>
       <c r="AC2" s="2" t="s">
         <v>44</v>
@@ -816,7 +806,7 @@
       <c r="AD2" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="AE2" s="5" t="s">
+      <c r="AE2" s="2" t="s">
         <v>39</v>
       </c>
       <c r="AF2" s="2" t="s">
@@ -874,7 +864,7 @@
       </c>
       <c r="J3" s="3">
         <f t="shared" si="1"/>
-        <v>28407</v>
+        <v>45528</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>39</v>
@@ -921,7 +911,7 @@
       <c r="Y3" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="Z3" s="5" t="s">
+      <c r="Z3" s="2" t="s">
         <v>39</v>
       </c>
       <c r="AA3" s="2" t="s">
@@ -929,7 +919,7 @@
       </c>
       <c r="AB3" s="6">
         <f t="shared" si="2"/>
-        <v>141</v>
+        <v>179</v>
       </c>
       <c r="AC3" s="2" t="s">
         <v>51</v>
@@ -937,7 +927,7 @@
       <c r="AD3" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="AE3" s="5" t="s">
+      <c r="AE3" s="2" t="s">
         <v>39</v>
       </c>
       <c r="AF3" s="2" t="s">
@@ -995,7 +985,7 @@
       </c>
       <c r="J4" s="3">
         <f t="shared" si="1"/>
-        <v>49122</v>
+        <v>12822</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>39</v>
@@ -1021,48 +1011,48 @@
       <c r="R4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="S4" s="2" t="s">
+      <c r="S4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="T4" s="6" t="s">
         <v>54</v>
       </c>
-      <c r="T4" s="6" t="s">
+      <c r="U4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="W4" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="U4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="V4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="W4" s="2" t="s">
+      <c r="X4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA4" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="X4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z4" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA4" s="2" t="s">
-        <v>57</v>
       </c>
       <c r="AB4" s="6">
         <f t="shared" si="2"/>
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="AC4" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="AD4" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="AD4" s="2" t="s">
+      <c r="AE4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF4" s="2" t="s">
         <v>59</v>
-      </c>
-      <c r="AE4" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF4" s="2" t="s">
-        <v>60</v>
       </c>
       <c r="AG4" s="2" t="s">
         <v>39</v>
@@ -1116,7 +1106,7 @@
       </c>
       <c r="J5" s="3">
         <f t="shared" si="1"/>
-        <v>43011</v>
+        <v>16105</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>39</v>
@@ -1143,10 +1133,10 @@
         <v>39</v>
       </c>
       <c r="S5" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="T5" s="6" t="s">
         <v>61</v>
-      </c>
-      <c r="T5" s="6" t="s">
-        <v>62</v>
       </c>
       <c r="U5" s="2" t="s">
         <v>39</v>
@@ -1163,27 +1153,27 @@
       <c r="Y5" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="Z5" s="5" t="s">
+      <c r="Z5" s="2" t="s">
         <v>39</v>
       </c>
       <c r="AA5" s="2" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AB5" s="6">
         <f t="shared" si="2"/>
-        <v>137</v>
+        <v>186</v>
       </c>
       <c r="AC5" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD5" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="AD5" s="2" t="s">
+      <c r="AE5" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF5" s="2" t="s">
         <v>65</v>
-      </c>
-      <c r="AE5" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF5" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="AG5" s="2" t="s">
         <v>39</v>
@@ -1237,7 +1227,7 @@
       </c>
       <c r="J6" s="3">
         <f t="shared" si="1"/>
-        <v>27140</v>
+        <v>32541</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>39</v>
@@ -1264,10 +1254,10 @@
         <v>39</v>
       </c>
       <c r="S6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="T6" s="6" t="s">
         <v>67</v>
-      </c>
-      <c r="T6" s="6" t="s">
-        <v>68</v>
       </c>
       <c r="U6" s="2" t="s">
         <v>39</v>
@@ -1284,27 +1274,27 @@
       <c r="Y6" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="Z6" s="5" t="s">
+      <c r="Z6" s="2" t="s">
         <v>39</v>
       </c>
       <c r="AA6" s="2" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="AB6" s="6">
         <f t="shared" si="2"/>
-        <v>195</v>
-      </c>
-      <c r="AC6" s="5" t="s">
+        <v>175</v>
+      </c>
+      <c r="AC6" s="2" t="s">
         <v>39</v>
       </c>
       <c r="AD6" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="AE6" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF6" s="2" t="s">
         <v>70</v>
-      </c>
-      <c r="AE6" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF6" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="AG6" s="2" t="s">
         <v>39</v>
@@ -1358,7 +1348,7 @@
       </c>
       <c r="J7" s="3">
         <f t="shared" si="1"/>
-        <v>55016</v>
+        <v>38377</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>39</v>
@@ -1385,47 +1375,47 @@
         <v>39</v>
       </c>
       <c r="S7" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="T7" s="6" t="s">
         <v>72</v>
       </c>
-      <c r="T7" s="6" t="s">
+      <c r="U7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="V7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="W7" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="X7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA7" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="U7" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="V7" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="W7" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="X7" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y7" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z7" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA7" s="2" t="s">
-        <v>74</v>
       </c>
       <c r="AB7" s="6">
         <f t="shared" si="2"/>
-        <v>174</v>
+        <v>159</v>
       </c>
       <c r="AC7" s="2" t="s">
         <v>44</v>
       </c>
       <c r="AD7" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="AE7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF7" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="AE7" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF7" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="AG7" s="2" t="s">
         <v>39</v>
@@ -1479,7 +1469,7 @@
       </c>
       <c r="J8" s="3">
         <f t="shared" si="1"/>
-        <v>48049</v>
+        <v>38290</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>39</v>
@@ -1509,7 +1499,7 @@
         <v>47</v>
       </c>
       <c r="T8" s="6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="U8" s="2" t="s">
         <v>39</v>
@@ -1526,27 +1516,27 @@
       <c r="Y8" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="Z8" s="5" t="s">
+      <c r="Z8" s="2" t="s">
         <v>39</v>
       </c>
       <c r="AA8" s="2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="AB8" s="6">
         <f t="shared" si="2"/>
-        <v>177</v>
+        <v>157</v>
       </c>
       <c r="AC8" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="AD8" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="AD8" s="2" t="s">
+      <c r="AE8" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF8" s="2" t="s">
         <v>80</v>
-      </c>
-      <c r="AE8" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF8" s="2" t="s">
-        <v>81</v>
       </c>
       <c r="AG8" s="2" t="s">
         <v>39</v>
@@ -1600,7 +1590,7 @@
       </c>
       <c r="J9" s="3">
         <f t="shared" si="1"/>
-        <v>49827</v>
+        <v>39633</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>39</v>
@@ -1627,10 +1617,10 @@
         <v>39</v>
       </c>
       <c r="S9" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="T9" s="6" t="s">
         <v>82</v>
-      </c>
-      <c r="T9" s="6" t="s">
-        <v>83</v>
       </c>
       <c r="U9" s="2" t="s">
         <v>39</v>
@@ -1647,27 +1637,27 @@
       <c r="Y9" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="Z9" s="5" t="s">
+      <c r="Z9" s="2" t="s">
         <v>39</v>
       </c>
       <c r="AA9" s="2" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="AB9" s="6">
         <f t="shared" si="2"/>
-        <v>127</v>
+        <v>197</v>
       </c>
       <c r="AC9" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="AD9" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="AE9" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF9" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="AE9" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF9" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="AG9" s="2" t="s">
         <v>39</v>
@@ -1721,7 +1711,7 @@
       </c>
       <c r="J10" s="3">
         <f t="shared" si="1"/>
-        <v>42871</v>
+        <v>46111</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>39</v>
@@ -1748,47 +1738,47 @@
         <v>39</v>
       </c>
       <c r="S10" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="T10" s="6" t="s">
         <v>87</v>
       </c>
-      <c r="T10" s="6" t="s">
+      <c r="U10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="V10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="W10" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="X10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA10" s="2" t="s">
         <v>88</v>
-      </c>
-      <c r="U10" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="V10" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="W10" s="2" t="s">
-        <v>56</v>
-      </c>
-      <c r="X10" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y10" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z10" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA10" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="AB10" s="6">
         <f t="shared" si="2"/>
-        <v>144</v>
+        <v>170</v>
       </c>
       <c r="AC10" s="2" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="AD10" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="AE10" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF10" s="2" t="s">
         <v>90</v>
-      </c>
-      <c r="AE10" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF10" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="AG10" s="2" t="s">
         <v>39</v>
@@ -1842,7 +1832,7 @@
       </c>
       <c r="J11" s="3">
         <f t="shared" si="1"/>
-        <v>24473</v>
+        <v>47346</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>39</v>
@@ -1869,10 +1859,10 @@
         <v>39</v>
       </c>
       <c r="S11" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="T11" s="6" t="s">
         <v>92</v>
-      </c>
-      <c r="T11" s="6" t="s">
-        <v>93</v>
       </c>
       <c r="U11" s="2" t="s">
         <v>39</v>
@@ -1889,27 +1879,27 @@
       <c r="Y11" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="Z11" s="5" t="s">
+      <c r="Z11" s="2" t="s">
         <v>39</v>
       </c>
       <c r="AA11" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="AB11" s="6">
         <f t="shared" si="2"/>
-        <v>190</v>
-      </c>
-      <c r="AC11" s="5" t="s">
+        <v>156</v>
+      </c>
+      <c r="AC11" s="2" t="s">
         <v>39</v>
       </c>
       <c r="AD11" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="AE11" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF11" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="AE11" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF11" s="2" t="s">
-        <v>96</v>
       </c>
       <c r="AG11" s="2" t="s">
         <v>39</v>

</xml_diff>

<commit_message>
login / equipes dinamicas / escritor correto arquivo
</commit_message>
<xml_diff>
--- a/Rotas.xlsx
+++ b/Rotas.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="408" uniqueCount="90">
   <si>
     <t>DATA</t>
   </si>
@@ -154,15 +154,9 @@
     <t>Jardim Eulina</t>
   </si>
   <si>
-    <t>São Paulo</t>
-  </si>
-  <si>
     <t>DAFBZ</t>
   </si>
   <si>
-    <t>Manutenção</t>
-  </si>
-  <si>
     <t>Travessa das Iridáceas</t>
   </si>
   <si>
@@ -178,103 +172,91 @@
     <t>ABERB</t>
   </si>
   <si>
+    <t>Rua José João de Souza</t>
+  </si>
+  <si>
+    <t>fundos</t>
+  </si>
+  <si>
+    <t>17023-862</t>
+  </si>
+  <si>
+    <t>Loteamento Mário Luiz Rodrigues do Prado</t>
+  </si>
+  <si>
+    <t>AERGE</t>
+  </si>
+  <si>
+    <t>Travessa Ângelo Betiol</t>
+  </si>
+  <si>
+    <t>terreo</t>
+  </si>
+  <si>
+    <t>09843-060</t>
+  </si>
+  <si>
+    <t>Batistini</t>
+  </si>
+  <si>
+    <t>ETYMN</t>
+  </si>
+  <si>
+    <t>Rua João Florêncio de Carvalho</t>
+  </si>
+  <si>
+    <t>17505-000</t>
+  </si>
+  <si>
+    <t>Jardim Eldorado</t>
+  </si>
+  <si>
+    <t>NSFGZ</t>
+  </si>
+  <si>
+    <t>Rua Dois</t>
+  </si>
+  <si>
+    <t>12043-613</t>
+  </si>
+  <si>
+    <t>Residencial Ouroville</t>
+  </si>
+  <si>
+    <t>RE5YZ</t>
+  </si>
+  <si>
+    <t>Rua Armando Brussolo</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>05048-050</t>
+  </si>
+  <si>
+    <t>Vila Romana</t>
+  </si>
+  <si>
+    <t>BSRTN</t>
+  </si>
+  <si>
+    <t>Avenida Ana Carolina de Barros Levy</t>
+  </si>
+  <si>
+    <t>13480-755</t>
+  </si>
+  <si>
+    <t>Centro</t>
+  </si>
+  <si>
+    <t>Presidente Prudente</t>
+  </si>
+  <si>
+    <t>NXVBN</t>
+  </si>
+  <si>
     <t>Troca Equipamento</t>
-  </si>
-  <si>
-    <t>Rua José João de Souza</t>
-  </si>
-  <si>
-    <t>fundos</t>
-  </si>
-  <si>
-    <t>17023-862</t>
-  </si>
-  <si>
-    <t>Loteamento Mário Luiz Rodrigues do Prado</t>
-  </si>
-  <si>
-    <t>São Bernardo do Campo</t>
-  </si>
-  <si>
-    <t>AERGE</t>
-  </si>
-  <si>
-    <t>Travessa Ângelo Betiol</t>
-  </si>
-  <si>
-    <t>terreo</t>
-  </si>
-  <si>
-    <t>09843-060</t>
-  </si>
-  <si>
-    <t>Batistini</t>
-  </si>
-  <si>
-    <t>Marília</t>
-  </si>
-  <si>
-    <t>ETYMN</t>
-  </si>
-  <si>
-    <t>Rua João Florêncio de Carvalho</t>
-  </si>
-  <si>
-    <t>17505-000</t>
-  </si>
-  <si>
-    <t>Jardim Eldorado</t>
-  </si>
-  <si>
-    <t>Taubaté</t>
-  </si>
-  <si>
-    <t>NSFGZ</t>
-  </si>
-  <si>
-    <t>Rua Dois</t>
-  </si>
-  <si>
-    <t>12043-613</t>
-  </si>
-  <si>
-    <t>Residencial Ouroville</t>
-  </si>
-  <si>
-    <t>RE5YZ</t>
-  </si>
-  <si>
-    <t>Rua Armando Brussolo</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>05048-050</t>
-  </si>
-  <si>
-    <t>Vila Romana</t>
-  </si>
-  <si>
-    <t>Limeira</t>
-  </si>
-  <si>
-    <t>BSRTN</t>
-  </si>
-  <si>
-    <t>Avenida Ana Carolina de Barros Levy</t>
-  </si>
-  <si>
-    <t>13480-755</t>
-  </si>
-  <si>
-    <t>Centro</t>
-  </si>
-  <si>
-    <t>Presidente Prudente</t>
-  </si>
-  <si>
-    <t>NXVBN</t>
   </si>
   <si>
     <t>Rua Antônio Pereira Telles</t>
@@ -341,7 +323,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -351,9 +333,6 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="3" numFmtId="1" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
     </xf>
     <xf quotePrefix="1" borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="center"/>
@@ -745,7 +724,7 @@
       </c>
       <c r="J2" s="3">
         <f t="shared" ref="J2:J11" si="1">RANDBETWEEN(11111,55555)</f>
-        <v>12910</v>
+        <v>24584</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>39</v>
@@ -769,10 +748,10 @@
       <c r="R2" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="S2" s="4" t="s">
+      <c r="S2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="T2" s="4" t="s">
         <v>41</v>
       </c>
       <c r="U2" s="2" t="s">
@@ -796,9 +775,9 @@
       <c r="AA2" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="AB2" s="6">
+      <c r="AB2" s="5">
         <f t="shared" ref="AB2:AB11" si="2">RANDBETWEEN(111,200)</f>
-        <v>148</v>
+        <v>189</v>
       </c>
       <c r="AC2" s="2" t="s">
         <v>44</v>
@@ -864,7 +843,7 @@
       </c>
       <c r="J3" s="3">
         <f t="shared" si="1"/>
-        <v>45528</v>
+        <v>33797</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>39</v>
@@ -891,47 +870,47 @@
         <v>39</v>
       </c>
       <c r="S3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="T3" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="T3" s="6" t="s">
+      <c r="U3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="V3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="W3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="X3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA3" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="U3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="V3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="W3" s="2" t="s">
+      <c r="AB3" s="5">
+        <f t="shared" si="2"/>
+        <v>157</v>
+      </c>
+      <c r="AC3" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="X3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA3" s="2" t="s">
+      <c r="AD3" s="2" t="s">
         <v>50</v>
       </c>
-      <c r="AB3" s="6">
-        <f t="shared" si="2"/>
-        <v>179</v>
-      </c>
-      <c r="AC3" s="2" t="s">
+      <c r="AE3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF3" s="2" t="s">
         <v>51</v>
-      </c>
-      <c r="AD3" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="AE3" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF3" s="2" t="s">
-        <v>53</v>
       </c>
       <c r="AG3" s="2" t="s">
         <v>39</v>
@@ -985,7 +964,7 @@
       </c>
       <c r="J4" s="3">
         <f t="shared" si="1"/>
-        <v>12822</v>
+        <v>38420</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>39</v>
@@ -1011,48 +990,48 @@
       <c r="R4" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="S4" s="4" t="s">
+      <c r="S4" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="T4" s="6" t="s">
+      <c r="T4" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="U4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="V4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="W4" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="X4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Y4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="Z4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AA4" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB4" s="5">
+        <f t="shared" si="2"/>
+        <v>140</v>
+      </c>
+      <c r="AC4" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="U4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="V4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="W4" s="2" t="s">
+      <c r="AD4" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="X4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Y4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="Z4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="AA4" s="2" t="s">
+      <c r="AE4" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="AF4" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="AB4" s="6">
-        <f t="shared" si="2"/>
-        <v>153</v>
-      </c>
-      <c r="AC4" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD4" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="AE4" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="AF4" s="2" t="s">
-        <v>59</v>
       </c>
       <c r="AG4" s="2" t="s">
         <v>39</v>
@@ -1106,7 +1085,7 @@
       </c>
       <c r="J5" s="3">
         <f t="shared" si="1"/>
-        <v>16105</v>
+        <v>31236</v>
       </c>
       <c r="K5" s="2" t="s">
         <v>39</v>
@@ -1133,10 +1112,10 @@
         <v>39</v>
       </c>
       <c r="S5" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="T5" s="6" t="s">
-        <v>61</v>
+        <v>40</v>
+      </c>
+      <c r="T5" s="5" t="s">
+        <v>57</v>
       </c>
       <c r="U5" s="2" t="s">
         <v>39</v>
@@ -1157,23 +1136,23 @@
         <v>39</v>
       </c>
       <c r="AA5" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="AB5" s="6">
+        <v>58</v>
+      </c>
+      <c r="AB5" s="5">
         <f t="shared" si="2"/>
-        <v>186</v>
+        <v>133</v>
       </c>
       <c r="AC5" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="AD5" s="2" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="AE5" s="2" t="s">
         <v>39</v>
       </c>
       <c r="AF5" s="2" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="AG5" s="2" t="s">
         <v>39</v>
@@ -1227,7 +1206,7 @@
       </c>
       <c r="J6" s="3">
         <f t="shared" si="1"/>
-        <v>32541</v>
+        <v>40678</v>
       </c>
       <c r="K6" s="2" t="s">
         <v>39</v>
@@ -1254,10 +1233,10 @@
         <v>39</v>
       </c>
       <c r="S6" s="2" t="s">
-        <v>66</v>
-      </c>
-      <c r="T6" s="6" t="s">
-        <v>67</v>
+        <v>40</v>
+      </c>
+      <c r="T6" s="5" t="s">
+        <v>62</v>
       </c>
       <c r="U6" s="2" t="s">
         <v>39</v>
@@ -1266,7 +1245,7 @@
         <v>39</v>
       </c>
       <c r="W6" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="X6" s="2" t="s">
         <v>39</v>
@@ -1278,23 +1257,23 @@
         <v>39</v>
       </c>
       <c r="AA6" s="2" t="s">
-        <v>68</v>
-      </c>
-      <c r="AB6" s="6">
+        <v>63</v>
+      </c>
+      <c r="AB6" s="5">
         <f t="shared" si="2"/>
-        <v>175</v>
+        <v>145</v>
       </c>
       <c r="AC6" s="2" t="s">
         <v>39</v>
       </c>
       <c r="AD6" s="2" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
       <c r="AE6" s="2" t="s">
         <v>39</v>
       </c>
       <c r="AF6" s="2" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="AG6" s="2" t="s">
         <v>39</v>
@@ -1348,7 +1327,7 @@
       </c>
       <c r="J7" s="3">
         <f t="shared" si="1"/>
-        <v>38377</v>
+        <v>26541</v>
       </c>
       <c r="K7" s="2" t="s">
         <v>39</v>
@@ -1375,10 +1354,10 @@
         <v>39</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="T7" s="6" t="s">
-        <v>72</v>
+        <v>40</v>
+      </c>
+      <c r="T7" s="5" t="s">
+        <v>66</v>
       </c>
       <c r="U7" s="2" t="s">
         <v>39</v>
@@ -1387,7 +1366,7 @@
         <v>39</v>
       </c>
       <c r="W7" s="2" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="X7" s="2" t="s">
         <v>39</v>
@@ -1399,23 +1378,23 @@
         <v>39</v>
       </c>
       <c r="AA7" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="AB7" s="6">
+        <v>67</v>
+      </c>
+      <c r="AB7" s="5">
         <f t="shared" si="2"/>
-        <v>159</v>
+        <v>129</v>
       </c>
       <c r="AC7" s="2" t="s">
         <v>44</v>
       </c>
       <c r="AD7" s="2" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="AE7" s="2" t="s">
         <v>39</v>
       </c>
       <c r="AF7" s="2" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="AG7" s="2" t="s">
         <v>39</v>
@@ -1469,7 +1448,7 @@
       </c>
       <c r="J8" s="3">
         <f t="shared" si="1"/>
-        <v>38290</v>
+        <v>17749</v>
       </c>
       <c r="K8" s="2" t="s">
         <v>39</v>
@@ -1496,10 +1475,10 @@
         <v>39</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="T8" s="6" t="s">
-        <v>76</v>
+        <v>40</v>
+      </c>
+      <c r="T8" s="5" t="s">
+        <v>70</v>
       </c>
       <c r="U8" s="2" t="s">
         <v>39</v>
@@ -1520,23 +1499,23 @@
         <v>39</v>
       </c>
       <c r="AA8" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="AB8" s="6">
+        <v>71</v>
+      </c>
+      <c r="AB8" s="5">
         <f t="shared" si="2"/>
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="AC8" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="AD8" s="2" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="AE8" s="2" t="s">
         <v>39</v>
       </c>
       <c r="AF8" s="2" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="AG8" s="2" t="s">
         <v>39</v>
@@ -1590,7 +1569,7 @@
       </c>
       <c r="J9" s="3">
         <f t="shared" si="1"/>
-        <v>39633</v>
+        <v>29648</v>
       </c>
       <c r="K9" s="2" t="s">
         <v>39</v>
@@ -1617,10 +1596,10 @@
         <v>39</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="T9" s="6" t="s">
-        <v>82</v>
+        <v>40</v>
+      </c>
+      <c r="T9" s="5" t="s">
+        <v>75</v>
       </c>
       <c r="U9" s="2" t="s">
         <v>39</v>
@@ -1629,7 +1608,7 @@
         <v>39</v>
       </c>
       <c r="W9" s="2" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="X9" s="2" t="s">
         <v>39</v>
@@ -1641,23 +1620,23 @@
         <v>39</v>
       </c>
       <c r="AA9" s="2" t="s">
-        <v>83</v>
-      </c>
-      <c r="AB9" s="6">
+        <v>76</v>
+      </c>
+      <c r="AB9" s="5">
         <f t="shared" si="2"/>
-        <v>197</v>
+        <v>128</v>
       </c>
       <c r="AC9" s="2" t="s">
-        <v>57</v>
+        <v>54</v>
       </c>
       <c r="AD9" s="2" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="AE9" s="2" t="s">
         <v>39</v>
       </c>
       <c r="AF9" s="2" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="AG9" s="2" t="s">
         <v>39</v>
@@ -1711,7 +1690,7 @@
       </c>
       <c r="J10" s="3">
         <f t="shared" si="1"/>
-        <v>46111</v>
+        <v>51565</v>
       </c>
       <c r="K10" s="2" t="s">
         <v>39</v>
@@ -1738,10 +1717,10 @@
         <v>39</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="T10" s="6" t="s">
-        <v>87</v>
+        <v>79</v>
+      </c>
+      <c r="T10" s="5" t="s">
+        <v>80</v>
       </c>
       <c r="U10" s="2" t="s">
         <v>39</v>
@@ -1750,7 +1729,7 @@
         <v>39</v>
       </c>
       <c r="W10" s="2" t="s">
-        <v>55</v>
+        <v>81</v>
       </c>
       <c r="X10" s="2" t="s">
         <v>39</v>
@@ -1762,23 +1741,23 @@
         <v>39</v>
       </c>
       <c r="AA10" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="AB10" s="6">
+        <v>82</v>
+      </c>
+      <c r="AB10" s="5">
         <f t="shared" si="2"/>
-        <v>170</v>
+        <v>127</v>
       </c>
       <c r="AC10" s="2" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="AD10" s="2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
       <c r="AE10" s="2" t="s">
         <v>39</v>
       </c>
       <c r="AF10" s="2" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="AG10" s="2" t="s">
         <v>39</v>
@@ -1832,7 +1811,7 @@
       </c>
       <c r="J11" s="3">
         <f t="shared" si="1"/>
-        <v>47346</v>
+        <v>27789</v>
       </c>
       <c r="K11" s="2" t="s">
         <v>39</v>
@@ -1859,10 +1838,10 @@
         <v>39</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="T11" s="6" t="s">
-        <v>92</v>
+        <v>85</v>
+      </c>
+      <c r="T11" s="5" t="s">
+        <v>86</v>
       </c>
       <c r="U11" s="2" t="s">
         <v>39</v>
@@ -1883,23 +1862,23 @@
         <v>39</v>
       </c>
       <c r="AA11" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="AB11" s="6">
+        <v>87</v>
+      </c>
+      <c r="AB11" s="5">
         <f t="shared" si="2"/>
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="AC11" s="2" t="s">
         <v>39</v>
       </c>
       <c r="AD11" s="2" t="s">
-        <v>94</v>
+        <v>88</v>
       </c>
       <c r="AE11" s="2" t="s">
         <v>39</v>
       </c>
       <c r="AF11" s="2" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="AG11" s="2" t="s">
         <v>39</v>

</xml_diff>